<commit_message>
Legend Updated with report data
</commit_message>
<xml_diff>
--- a/Resources/Effect of twist on Cp.xlsx
+++ b/Resources/Effect of twist on Cp.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="28660" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="-24" yWindow="-24" windowWidth="28656" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -103,6 +103,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +142,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -167,10 +167,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0967778928584798"/>
-          <c:y val="0.0999040767386091"/>
-          <c:w val="0.772789223454834"/>
-          <c:h val="0.878521939953811"/>
+          <c:x val="9.6777892858479819E-2"/>
+          <c:y val="9.9904076738609141E-2"/>
+          <c:w val="0.77278922345483425"/>
+          <c:h val="0.87852193995381112"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -193,40 +193,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.560593</c:v>
+                  <c:v>0.56059300000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.603885</c:v>
+                  <c:v>0.60388500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.647083</c:v>
+                  <c:v>0.64708299999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.690178</c:v>
+                  <c:v>0.69017799999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.733161</c:v>
+                  <c:v>0.73316099999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.776023</c:v>
+                  <c:v>0.77602300000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.818755</c:v>
+                  <c:v>0.81875500000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.861348</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.903794</c:v>
+                  <c:v>0.90379399999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.946083</c:v>
+                  <c:v>0.94608300000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.988207</c:v>
+                  <c:v>0.98820699999999995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.030158</c:v>
+                  <c:v>1.0301579999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -238,31 +238,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-0.0368</c:v>
+                  <c:v>-3.6799999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.048</c:v>
+                  <c:v>-4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0577</c:v>
+                  <c:v>-5.7700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0662</c:v>
+                  <c:v>-6.6199999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0737</c:v>
+                  <c:v>-7.3700000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.0804</c:v>
+                  <c:v>-8.0399999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.0864</c:v>
+                  <c:v>-8.6400000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.0918</c:v>
+                  <c:v>-9.1800000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0968</c:v>
+                  <c:v>-9.6799999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>-0.1012</c:v>
@@ -295,37 +295,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.611094</c:v>
+                  <c:v>0.61109400000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.654039</c:v>
+                  <c:v>0.65403900000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.696866</c:v>
+                  <c:v>0.69686599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.739569</c:v>
+                  <c:v>0.73956900000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.782136</c:v>
+                  <c:v>0.78213600000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.824561</c:v>
+                  <c:v>0.82456099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.866834</c:v>
+                  <c:v>0.86683399999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.908946</c:v>
+                  <c:v>0.90894600000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.950889</c:v>
+                  <c:v>0.95088899999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.992655</c:v>
+                  <c:v>0.99265499999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.034234</c:v>
+                  <c:v>1.0342340000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.07562</c:v>
@@ -340,7 +340,7 @@
                   <c:v>1.198529</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.239056</c:v>
+                  <c:v>1.2390559999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.27935</c:v>
@@ -355,37 +355,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-0.0252</c:v>
+                  <c:v>-2.52E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.0364</c:v>
+                  <c:v>-3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0462</c:v>
+                  <c:v>-4.6199999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0549</c:v>
+                  <c:v>-5.4899999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0626</c:v>
+                  <c:v>-6.2600000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.0696</c:v>
+                  <c:v>-6.9599999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.0758</c:v>
+                  <c:v>-7.5800000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.0815</c:v>
+                  <c:v>-8.1500000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0867</c:v>
+                  <c:v>-8.6699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0915</c:v>
+                  <c:v>-9.1499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.0959</c:v>
+                  <c:v>-9.5899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>-0.1</c:v>
@@ -394,7 +394,7 @@
                   <c:v>-0.1038</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.1073</c:v>
+                  <c:v>-0.10730000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>-0.1106</c:v>
@@ -427,52 +427,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.617583</c:v>
+                  <c:v>0.61758299999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.660219</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.702726</c:v>
+                  <c:v>0.70272599999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.745094</c:v>
+                  <c:v>0.74509400000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.787315</c:v>
+                  <c:v>0.78731499999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.829381</c:v>
+                  <c:v>0.82938100000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.871282</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.913011</c:v>
+                  <c:v>0.91301100000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.954559</c:v>
+                  <c:v>0.95455900000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.995918</c:v>
+                  <c:v>0.99591799999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.037079</c:v>
+                  <c:v>1.0370790000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.078035</c:v>
+                  <c:v>1.0780350000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.118778</c:v>
+                  <c:v>1.1187780000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.159299</c:v>
+                  <c:v>1.1592990000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1.199592</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.239648</c:v>
+                  <c:v>1.2396480000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,49 +484,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-0.0033</c:v>
+                  <c:v>-3.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.0159</c:v>
+                  <c:v>-1.5900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0269</c:v>
+                  <c:v>-2.69E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0367</c:v>
+                  <c:v>-3.6700000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0454</c:v>
+                  <c:v>-4.5400000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.0533</c:v>
+                  <c:v>-5.33E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.0604</c:v>
+                  <c:v>-6.0400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.0668</c:v>
+                  <c:v>-6.6799999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0727</c:v>
+                  <c:v>-7.2700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0781</c:v>
+                  <c:v>-7.8100000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.0831</c:v>
+                  <c:v>-8.3099999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.0878</c:v>
+                  <c:v>-8.7800000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.0921</c:v>
+                  <c:v>-9.2100000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.0961</c:v>
+                  <c:v>-9.6100000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.0998</c:v>
+                  <c:v>-9.98E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>-0.1033</c:v>
@@ -553,70 +553,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.312259</c:v>
+                  <c:v>0.31225900000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.355666</c:v>
+                  <c:v>0.35566599999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.399012</c:v>
+                  <c:v>0.39901199999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.442289</c:v>
+                  <c:v>0.44228899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.485488</c:v>
+                  <c:v>0.48548799999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.528599</c:v>
+                  <c:v>0.52859900000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.571614</c:v>
+                  <c:v>0.57161399999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.614523</c:v>
+                  <c:v>0.61452300000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.657318</c:v>
+                  <c:v>0.65731799999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.699989</c:v>
+                  <c:v>0.69998899999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.742528</c:v>
+                  <c:v>0.74252799999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.784927</c:v>
+                  <c:v>0.78492700000000004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.827176</c:v>
+                  <c:v>0.82717600000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.869266</c:v>
+                  <c:v>0.86926599999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.91119</c:v>
+                  <c:v>0.91119000000000006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.952939</c:v>
+                  <c:v>0.95293899999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.994505</c:v>
+                  <c:v>0.99450499999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.035878</c:v>
+                  <c:v>1.0358780000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.077052</c:v>
+                  <c:v>1.0770519999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1.118017</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.158767</c:v>
+                  <c:v>1.1587670000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.199293</c:v>
+                  <c:v>1.1992929999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1.239587</c:v>
@@ -625,7 +625,7 @@
                   <c:v>1.279641</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.319449</c:v>
+                  <c:v>1.3194490000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -637,64 +637,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.1606</c:v>
+                  <c:v>0.16059999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.1174</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0835</c:v>
+                  <c:v>8.3500000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0564</c:v>
+                  <c:v>5.6399999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.034</c:v>
+                  <c:v>3.4000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0153</c:v>
+                  <c:v>1.5299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.0005</c:v>
+                  <c:v>-5.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.0142</c:v>
+                  <c:v>-1.4200000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0261</c:v>
+                  <c:v>-2.6100000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0365</c:v>
+                  <c:v>-3.6499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.0457</c:v>
+                  <c:v>-4.5699999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.054</c:v>
+                  <c:v>-5.3999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.0614</c:v>
+                  <c:v>-6.1400000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.0681</c:v>
+                  <c:v>-6.8099999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.0741</c:v>
+                  <c:v>-7.4099999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.0797</c:v>
+                  <c:v>-7.9699999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.0848</c:v>
+                  <c:v>-8.48E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.0895</c:v>
+                  <c:v>-8.9499999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.0938</c:v>
+                  <c:v>-9.3799999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.0979</c:v>
+                  <c:v>-9.7900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>-0.1017</c:v>
@@ -715,11 +715,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="507363288"/>
-        <c:axId val="514862632"/>
+        <c:axId val="65442176"/>
+        <c:axId val="65443712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="507363288"/>
+        <c:axId val="65442176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -728,22 +728,22 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="514862632"/>
+        <c:crossAx val="65443712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="514862632"/>
+        <c:axId val="65443712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-0.05"/>
-          <c:min val="-0.15"/>
+          <c:min val="-0.15000000000000002"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="507363288"/>
+        <c:crossAx val="65442176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -755,10 +755,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.777761458502315"/>
-          <c:y val="0.248523197190279"/>
-          <c:w val="0.136660094588018"/>
-          <c:h val="0.173457202741744"/>
+          <c:x val="0.77776145850231515"/>
+          <c:y val="0.24852319719027904"/>
+          <c:w val="0.13666009458801801"/>
+          <c:h val="0.17345720274174403"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -766,7 +766,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -776,7 +776,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -818,31 +817,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.517477</c:v>
+                  <c:v>0.51747699999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.560304</c:v>
+                  <c:v>0.56030400000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.603048</c:v>
+                  <c:v>0.60304800000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.645701</c:v>
+                  <c:v>0.64570099999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.688254</c:v>
+                  <c:v>0.68825400000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.730699</c:v>
+                  <c:v>0.73069899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.773027</c:v>
+                  <c:v>0.77302700000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.815231</c:v>
+                  <c:v>0.81523100000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8573</c:v>
+                  <c:v>0.85729999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -854,31 +853,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.6772</c:v>
+                  <c:v>0.67720000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6584</c:v>
+                  <c:v>0.65839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6423</c:v>
+                  <c:v>0.64229999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6283</c:v>
+                  <c:v>0.62829999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6161</c:v>
+                  <c:v>0.61609999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6054</c:v>
+                  <c:v>0.60540000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5959</c:v>
+                  <c:v>0.59589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5875</c:v>
+                  <c:v>0.58750000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5799</c:v>
+                  <c:v>0.57989999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -902,40 +901,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.58323</c:v>
+                  <c:v>0.58323000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.625983</c:v>
+                  <c:v>0.62598299999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.668634</c:v>
+                  <c:v>0.66863399999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.711175</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.753598</c:v>
+                  <c:v>0.75359799999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.795893</c:v>
+                  <c:v>0.79589299999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.838053</c:v>
+                  <c:v>0.83805300000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.880069</c:v>
+                  <c:v>0.88006899999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.921932</c:v>
+                  <c:v>0.92193199999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.963635</c:v>
+                  <c:v>0.96363500000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.005169</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.046526</c:v>
+                  <c:v>1.0465260000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -947,40 +946,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.6087</c:v>
+                  <c:v>0.60870000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5967</c:v>
+                  <c:v>0.59670000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5862</c:v>
+                  <c:v>0.58620000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5771</c:v>
+                  <c:v>0.57709999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.569</c:v>
+                  <c:v>0.56899999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5619</c:v>
+                  <c:v>0.56189999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5555</c:v>
+                  <c:v>0.55549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5498</c:v>
+                  <c:v>0.54979999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5447</c:v>
+                  <c:v>0.54469999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5358</c:v>
+                  <c:v>0.53580000000000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.532</c:v>
+                  <c:v>0.53200000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,37 +1003,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.607482</c:v>
+                  <c:v>0.60748199999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.650127</c:v>
+                  <c:v>0.65012700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.692661</c:v>
+                  <c:v>0.69266099999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.735073</c:v>
+                  <c:v>0.73507299999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.777357</c:v>
+                  <c:v>0.77735699999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.819504</c:v>
+                  <c:v>0.81950400000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.861505</c:v>
+                  <c:v>0.86150499999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.903352</c:v>
+                  <c:v>0.90335200000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.945036</c:v>
+                  <c:v>0.94503599999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.98655</c:v>
+                  <c:v>0.98655000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.027886</c:v>
+                  <c:v>1.0278860000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.069035</c:v>
@@ -1043,19 +1042,19 @@
                   <c:v>1.10999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.150743</c:v>
+                  <c:v>1.1507430000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.191285</c:v>
+                  <c:v>1.1912849999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.23161</c:v>
+                  <c:v>1.2316100000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.27171</c:v>
+                  <c:v>1.2717099999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.311578</c:v>
+                  <c:v>1.3115779999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1067,58 +1066,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.5627</c:v>
+                  <c:v>0.56269999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5543</c:v>
+                  <c:v>0.55430000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5469</c:v>
+                  <c:v>0.54690000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5405</c:v>
+                  <c:v>0.54049999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5349</c:v>
+                  <c:v>0.53490000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5298</c:v>
+                  <c:v>0.52980000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5253</c:v>
+                  <c:v>0.52529999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5213</c:v>
+                  <c:v>0.52129999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5177</c:v>
+                  <c:v>0.51770000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5144</c:v>
+                  <c:v>0.51439999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5115</c:v>
+                  <c:v>0.51149999999999995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5088</c:v>
+                  <c:v>0.50880000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5064</c:v>
+                  <c:v>0.50639999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.5042</c:v>
+                  <c:v>0.50419999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.5022</c:v>
+                  <c:v>0.50219999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5004</c:v>
+                  <c:v>0.50039999999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.4988</c:v>
+                  <c:v>0.49880000000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.4973</c:v>
+                  <c:v>0.49730000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1142,67 +1141,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.353884</c:v>
+                  <c:v>0.35388399999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.397035</c:v>
+                  <c:v>0.39703500000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.440128</c:v>
+                  <c:v>0.44012800000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.483153</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.526104</c:v>
+                  <c:v>0.52610400000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56897</c:v>
+                  <c:v>0.56896999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.611743</c:v>
+                  <c:v>0.61174300000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.654415</c:v>
+                  <c:v>0.65441499999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.696976</c:v>
+                  <c:v>0.69697600000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.739418</c:v>
+                  <c:v>0.73941800000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.781733</c:v>
+                  <c:v>0.78173300000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.823912</c:v>
+                  <c:v>0.82391199999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.865947</c:v>
+                  <c:v>0.86594700000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.907829</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.949551</c:v>
+                  <c:v>0.94955100000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.991103</c:v>
+                  <c:v>0.99110299999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.032479</c:v>
+                  <c:v>1.0324789999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.073669</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.114666</c:v>
+                  <c:v>1.1146659999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1.155462</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.196049</c:v>
+                  <c:v>1.1960489999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1214,77 +1213,77 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.6877</c:v>
+                  <c:v>0.68769999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6599</c:v>
+                  <c:v>0.65990000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6377</c:v>
+                  <c:v>0.63770000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6194</c:v>
+                  <c:v>0.61939999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6042</c:v>
+                  <c:v>0.60419999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5913</c:v>
+                  <c:v>0.59130000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5803</c:v>
+                  <c:v>0.58030000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5707</c:v>
+                  <c:v>0.57069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5624</c:v>
+                  <c:v>0.56240000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5551</c:v>
+                  <c:v>0.55510000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5486</c:v>
+                  <c:v>0.54859999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5428</c:v>
+                  <c:v>0.54279999999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5377</c:v>
+                  <c:v>0.53769999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.5331</c:v>
+                  <c:v>0.53310000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.5289</c:v>
+                  <c:v>0.52890000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5251</c:v>
+                  <c:v>0.52510000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.5217</c:v>
+                  <c:v>0.52170000000000005</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5186</c:v>
+                  <c:v>0.51859999999999995</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.5158</c:v>
+                  <c:v>0.51580000000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.5133</c:v>
+                  <c:v>0.51329999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.5109</c:v>
+                  <c:v>0.51090000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="514929336"/>
-        <c:axId val="514932552"/>
+        <c:axId val="65479808"/>
+        <c:axId val="65481344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="514929336"/>
+        <c:axId val="65479808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1293,22 +1292,22 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="514932552"/>
+        <c:crossAx val="65481344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="514932552"/>
+        <c:axId val="65481344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.6"/>
+          <c:max val="0.60000000000000009"/>
           <c:min val="0.5"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="514929336"/>
+        <c:crossAx val="65479808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -1322,7 +1321,263 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10109711286089239"/>
+          <c:y val="4.6770924467774859E-2"/>
+          <c:w val="0.74718197725284341"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$52:$S$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$52:$T$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$28:$I$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.33649999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.35E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6.1499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.126</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.182</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.23099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.27449999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.313</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.379</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.40749999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.4335</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.45749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.47949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.51900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.53649999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.55299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.56849999999999989</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.58299999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.39493699999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43832900000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.481651</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.524891</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56804200000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61109400000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65403900000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69686599999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.73956900000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.78213600000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.82456099999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.86683399999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.90894600000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95088899999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99265499999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0342340000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.07562</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.116803</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.157775</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.198529</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2390559999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.27935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="125702912"/>
+        <c:axId val="125701120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="125702912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125701120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="125701120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125702912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1385,6 +1640,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1712,15 +1997,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A8:H197"/>
+  <dimension ref="A8:I197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="S72" sqref="S51:T72"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28:I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6"/>
   <sheetData>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
@@ -1896,7 +2181,7 @@
         <v>-7.3700000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:9">
       <c r="B17">
         <v>0.5</v>
       </c>
@@ -1919,7 +2204,7 @@
         <v>-8.0399999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:9">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1942,7 +2227,7 @@
         <v>-8.6400000000000005E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:9">
       <c r="B19">
         <v>1.5</v>
       </c>
@@ -1965,7 +2250,7 @@
         <v>-9.1800000000000007E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:9">
       <c r="B20">
         <v>2</v>
       </c>
@@ -1988,7 +2273,7 @@
         <v>-9.6799999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:9">
       <c r="B21">
         <v>2.5</v>
       </c>
@@ -2011,7 +2296,7 @@
         <v>-0.1012</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:9">
       <c r="B22">
         <v>3</v>
       </c>
@@ -2034,7 +2319,7 @@
         <v>-0.1053</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:9">
       <c r="B23">
         <v>3.5</v>
       </c>
@@ -2057,12 +2342,12 @@
         <v>-0.1091</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:9">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -2085,7 +2370,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -2108,7 +2393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:9">
       <c r="B28">
         <v>-2</v>
       </c>
@@ -2130,8 +2415,12 @@
       <c r="H28">
         <v>6.7299999999999999E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:8">
+      <c r="I28">
+        <f>H28/0.2</f>
+        <v>0.33649999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
       <c r="B29">
         <v>-1.5</v>
       </c>
@@ -2153,8 +2442,12 @@
       <c r="H29">
         <v>4.1500000000000002E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:8">
+      <c r="I29">
+        <f t="shared" ref="I29:I49" si="0">H29/0.2</f>
+        <v>0.20749999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
       <c r="B30">
         <v>-1</v>
       </c>
@@ -2176,8 +2469,12 @@
       <c r="H30">
         <v>2.0299999999999999E-2</v>
       </c>
-    </row>
-    <row r="31" spans="2:8">
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0.10149999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
       <c r="B31">
         <v>-0.5</v>
       </c>
@@ -2199,8 +2496,12 @@
       <c r="H31">
         <v>2.7000000000000001E-3</v>
       </c>
-    </row>
-    <row r="32" spans="2:8">
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>1.35E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
       <c r="B32">
         <v>0</v>
       </c>
@@ -2222,8 +2523,12 @@
       <c r="H32">
         <v>-1.23E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:8">
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>-6.1499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
       <c r="B33">
         <v>0.5</v>
       </c>
@@ -2245,8 +2550,12 @@
       <c r="H33">
         <v>-2.52E-2</v>
       </c>
-    </row>
-    <row r="34" spans="2:8">
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>-0.126</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
       <c r="B34">
         <v>1</v>
       </c>
@@ -2268,8 +2577,12 @@
       <c r="H34">
         <v>-3.6400000000000002E-2</v>
       </c>
-    </row>
-    <row r="35" spans="2:8">
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>-0.182</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
       <c r="B35">
         <v>1.5</v>
       </c>
@@ -2291,8 +2604,12 @@
       <c r="H35">
         <v>-4.6199999999999998E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:8">
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>-0.23099999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
       <c r="B36">
         <v>2</v>
       </c>
@@ -2314,8 +2631,12 @@
       <c r="H36">
         <v>-5.4899999999999997E-2</v>
       </c>
-    </row>
-    <row r="37" spans="2:8">
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>-0.27449999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
       <c r="B37">
         <v>2.5</v>
       </c>
@@ -2337,8 +2658,12 @@
       <c r="H37">
         <v>-6.2600000000000003E-2</v>
       </c>
-    </row>
-    <row r="38" spans="2:8">
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>-0.313</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
       <c r="B38">
         <v>3</v>
       </c>
@@ -2360,8 +2685,12 @@
       <c r="H38">
         <v>-6.9599999999999995E-2</v>
       </c>
-    </row>
-    <row r="39" spans="2:8">
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>-0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
       <c r="B39">
         <v>3.5</v>
       </c>
@@ -2383,8 +2712,12 @@
       <c r="H39">
         <v>-7.5800000000000006E-2</v>
       </c>
-    </row>
-    <row r="40" spans="2:8">
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>-0.379</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
       <c r="B40">
         <v>4</v>
       </c>
@@ -2406,8 +2739,12 @@
       <c r="H40">
         <v>-8.1500000000000003E-2</v>
       </c>
-    </row>
-    <row r="41" spans="2:8">
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>-0.40749999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
       <c r="B41">
         <v>4.5</v>
       </c>
@@ -2429,8 +2766,12 @@
       <c r="H41">
         <v>-8.6699999999999999E-2</v>
       </c>
-    </row>
-    <row r="42" spans="2:8">
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>-0.4335</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
       <c r="B42">
         <v>5</v>
       </c>
@@ -2452,8 +2793,12 @@
       <c r="H42">
         <v>-9.1499999999999998E-2</v>
       </c>
-    </row>
-    <row r="43" spans="2:8">
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>-0.45749999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
       <c r="B43">
         <v>5.5</v>
       </c>
@@ -2475,8 +2820,12 @@
       <c r="H43">
         <v>-9.5899999999999999E-2</v>
       </c>
-    </row>
-    <row r="44" spans="2:8">
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>-0.47949999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
       <c r="B44">
         <v>6</v>
       </c>
@@ -2498,8 +2847,12 @@
       <c r="H44">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="45" spans="2:8">
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9">
       <c r="B45">
         <v>6.5</v>
       </c>
@@ -2521,8 +2874,12 @@
       <c r="H45">
         <v>-0.1038</v>
       </c>
-    </row>
-    <row r="46" spans="2:8">
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>-0.51900000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
       <c r="B46">
         <v>7</v>
       </c>
@@ -2544,8 +2901,12 @@
       <c r="H46">
         <v>-0.10730000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="2:8">
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>-0.53649999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9">
       <c r="B47">
         <v>7.5</v>
       </c>
@@ -2567,8 +2928,12 @@
       <c r="H47">
         <v>-0.1106</v>
       </c>
-    </row>
-    <row r="48" spans="2:8">
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>-0.55299999999999994</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9">
       <c r="B48">
         <v>8</v>
       </c>
@@ -2590,8 +2955,12 @@
       <c r="H48">
         <v>-0.1137</v>
       </c>
-    </row>
-    <row r="49" spans="2:8">
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>-0.56849999999999989</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
       <c r="B49">
         <v>8.5</v>
       </c>
@@ -2613,13 +2982,17 @@
       <c r="H49">
         <v>-0.1166</v>
       </c>
-    </row>
-    <row r="51" spans="2:8">
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>-0.58299999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
       <c r="B51" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="2:9">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -2642,7 +3015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="2:8">
+    <row r="53" spans="2:9">
       <c r="B53" t="s">
         <v>7</v>
       </c>
@@ -2665,7 +3038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:8">
+    <row r="54" spans="2:9">
       <c r="B54">
         <v>-2</v>
       </c>
@@ -2688,7 +3061,7 @@
         <v>0.16059999999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:8">
+    <row r="55" spans="2:9">
       <c r="B55">
         <v>-1.5</v>
       </c>
@@ -2711,7 +3084,7 @@
         <v>0.1174</v>
       </c>
     </row>
-    <row r="56" spans="2:8">
+    <row r="56" spans="2:9">
       <c r="B56">
         <v>-1</v>
       </c>
@@ -2734,7 +3107,7 @@
         <v>8.3500000000000005E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:8">
+    <row r="57" spans="2:9">
       <c r="B57">
         <v>-0.5</v>
       </c>
@@ -2757,7 +3130,7 @@
         <v>5.6399999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:8">
+    <row r="58" spans="2:9">
       <c r="B58">
         <v>0</v>
       </c>
@@ -2780,7 +3153,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:8">
+    <row r="59" spans="2:9">
       <c r="B59">
         <v>0.5</v>
       </c>
@@ -2803,7 +3176,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:8">
+    <row r="60" spans="2:9">
       <c r="B60">
         <v>1</v>
       </c>
@@ -2826,7 +3199,7 @@
         <v>-5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="61" spans="2:8">
+    <row r="61" spans="2:9">
       <c r="B61">
         <v>1.5</v>
       </c>
@@ -2849,7 +3222,7 @@
         <v>-1.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:8">
+    <row r="62" spans="2:9">
       <c r="B62">
         <v>2</v>
       </c>
@@ -2872,7 +3245,7 @@
         <v>-2.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:8">
+    <row r="63" spans="2:9">
       <c r="B63">
         <v>2.5</v>
       </c>
@@ -2895,7 +3268,7 @@
         <v>-3.6499999999999998E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:8">
+    <row r="64" spans="2:9">
       <c r="B64">
         <v>3</v>
       </c>

</xml_diff>